<commit_message>
TAC SP files; BW Rmd
</commit_message>
<xml_diff>
--- a/Output/statistics.xlsx
+++ b/Output/statistics.xlsx
@@ -8,13 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/Acclim_Dynamics/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDEE267-696F-B847-BCB3-72941F3E3C7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62F8046-7CC1-2943-B290-DB63A5CAF139}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="460" windowWidth="28020" windowHeight="19060" activeTab="1" xr2:uid="{01A92F3B-E9E7-3E4F-8152-3E4436457870}"/>
+    <workbookView xWindow="72000" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{01A92F3B-E9E7-3E4F-8152-3E4436457870}"/>
   </bookViews>
   <sheets>
     <sheet name="Survivorship" sheetId="1" r:id="rId1"/>
     <sheet name="Respiration_Photosynthesis" sheetId="2" r:id="rId2"/>
+    <sheet name="Bleaching_Score" sheetId="3" r:id="rId3"/>
+    <sheet name="Buoyant_Weight" sheetId="5" r:id="rId4"/>
+    <sheet name="Chlorophyll" sheetId="6" r:id="rId5"/>
+    <sheet name="Tissue_Biomass" sheetId="7" r:id="rId6"/>
+    <sheet name="Total_Antioxidant_Capacity" sheetId="8" r:id="rId7"/>
+    <sheet name="Protein" sheetId="9" r:id="rId8"/>
+    <sheet name="ITS2" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="51">
   <si>
     <t>Species</t>
   </si>
@@ -109,17 +116,97 @@
   </si>
   <si>
     <t>Respiration Rate</t>
+  </si>
+  <si>
+    <t>Stats are for the set with the 10 missing corals</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>Bleaching Score</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>Timepoint</t>
+  </si>
+  <si>
+    <t>Temperature:CO2</t>
+  </si>
+  <si>
+    <t>Temperature:Timepoint</t>
+  </si>
+  <si>
+    <t>CO2:Timepoint</t>
+  </si>
+  <si>
+    <t>Temperature:Species</t>
+  </si>
+  <si>
+    <t>CO2:Species</t>
+  </si>
+  <si>
+    <t>Timepoint:Species</t>
+  </si>
+  <si>
+    <t>Temperature:CO2:Timepoint</t>
+  </si>
+  <si>
+    <t>Temperature:CO2:Species</t>
+  </si>
+  <si>
+    <t>Temperature:Timepoint:Species</t>
+  </si>
+  <si>
+    <t>CO2:Timepoint:Species</t>
+  </si>
+  <si>
+    <t>Temperature:CO2:Timepoint:Species</t>
+  </si>
+  <si>
+    <t>survfit() in R</t>
+  </si>
+  <si>
+    <t>All above ANOVA following this code: Mcap.Rdark.aov &lt;- aov(Rdark_umol.cm2.hr ~ pCO2.Trt*Tmp.Trt*Date.x, data = Mcap.All)</t>
+  </si>
+  <si>
+    <t>&lt; 2E-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mod1 &lt;- aov(sqrt(Bleaching.Score+200) ~ Temperature*CO2*Timepoint*Species, data=Color.Score) #run an ANOVA </t>
+  </si>
+  <si>
+    <t>Last updated 20200904</t>
+  </si>
+  <si>
+    <t>Buoyant Weight</t>
+  </si>
+  <si>
+    <t>&lt; 2e-16</t>
+  </si>
+  <si>
+    <t>Last updated 20200930</t>
+  </si>
+  <si>
+    <t>mod1 &lt;- aov(mg.d.cm2 ~ Temperature*CO2*TimePoint*Species, data=data.long)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="171" formatCode="0.0000"/>
-    <numFmt numFmtId="172" formatCode="0.000"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -147,6 +234,14 @@
       <b/>
       <i/>
       <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -441,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -450,15 +545,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
@@ -472,6 +558,49 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -481,14 +610,42 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962EE7B6-A275-B345-99BE-8351465C90D0}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -819,16 +976,16 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="10">
         <v>0.18</v>
       </c>
       <c r="C2" s="2"/>
@@ -837,7 +994,7 @@
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -850,6 +1007,11 @@
       </c>
       <c r="B6">
         <v>20200903</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -859,653 +1021,2126 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E5E69C-11A6-AE47-A42F-E27125390009}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.83203125" customWidth="1"/>
+    <col min="9" max="9" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:15" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="26"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="50"/>
+      <c r="I1" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="50"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="22"/>
-      <c r="B3" s="23" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="53"/>
+      <c r="I2" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="53"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="G3" s="18"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="18"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="14">
-        <v>1</v>
-      </c>
-      <c r="C4" s="14">
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11">
         <v>0.76200000000000001</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="11">
         <v>0.76200000000000001</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="11">
         <v>4.9450000000000003</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="13">
         <v>2.7699999999999999E-2</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="I4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="11">
+        <v>1</v>
+      </c>
+      <c r="K4" s="11">
+        <v>7.1800000000000003E-2</v>
+      </c>
+      <c r="L4" s="11">
+        <v>7.1800000000000003E-2</v>
+      </c>
+      <c r="M4" s="11">
+        <v>3.742</v>
+      </c>
+      <c r="N4" s="32">
+        <v>5.5019999999999999E-2</v>
+      </c>
+      <c r="O4" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="14">
-        <v>1</v>
-      </c>
-      <c r="C5" s="31">
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
+      <c r="C5" s="25">
         <v>8.2200000000000006</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="25">
         <v>8.2200000000000006</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="11">
         <v>53.338999999999999</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="14">
         <v>1.7199999999999999E-11</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="I5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="11">
+        <v>1</v>
+      </c>
+      <c r="K5" s="24">
+        <v>0.18870000000000001</v>
+      </c>
+      <c r="L5" s="24">
+        <v>0.18870000000000001</v>
+      </c>
+      <c r="M5" s="11">
+        <v>9.8309999999999995</v>
+      </c>
+      <c r="N5" s="15">
+        <v>2.0799999999999998E-3</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="14">
-        <v>1</v>
-      </c>
-      <c r="C6" s="14">
+      <c r="B6" s="11">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11">
         <v>8.7390000000000008</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="11">
         <v>8.7390000000000008</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="11">
         <v>56.709000000000003</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="14">
         <v>4.9599999999999999E-12</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="I6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="11">
+        <v>1</v>
+      </c>
+      <c r="K6" s="11">
+        <v>5.0200000000000002E-2</v>
+      </c>
+      <c r="L6" s="11">
+        <v>5.0200000000000002E-2</v>
+      </c>
+      <c r="M6" s="11">
+        <v>2.6139999999999999</v>
+      </c>
+      <c r="N6" s="32">
+        <v>0.10811</v>
+      </c>
+      <c r="O6" s="7"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="14">
-        <v>1</v>
-      </c>
-      <c r="C7" s="14">
+      <c r="B7" s="11">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="11">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="11">
         <v>2.3E-2</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="11">
         <v>0.88049999999999995</v>
       </c>
       <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="I7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="11">
+        <v>1</v>
+      </c>
+      <c r="K7" s="11">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="L7" s="11">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="M7" s="11">
+        <v>0.379</v>
+      </c>
+      <c r="N7" s="30">
+        <v>0.53907000000000005</v>
+      </c>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="14">
-        <v>1</v>
-      </c>
-      <c r="C8" s="14">
+      <c r="B8" s="11">
+        <v>1</v>
+      </c>
+      <c r="C8" s="11">
         <v>0.19600000000000001</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="11">
         <v>0.19600000000000001</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="11">
         <v>1.274</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="24">
         <v>0.26100000000000001</v>
       </c>
       <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="I8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="11">
+        <v>1</v>
+      </c>
+      <c r="K8" s="11">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="L8" s="11">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="M8" s="11">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="N8" s="30">
+        <v>0.8296</v>
+      </c>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="14">
-        <v>1</v>
-      </c>
-      <c r="C9" s="14">
+      <c r="B9" s="11">
+        <v>1</v>
+      </c>
+      <c r="C9" s="11">
         <v>4.0570000000000004</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="11">
         <v>4.0570000000000004</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="11">
         <v>26.326000000000001</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="14">
         <v>9.1100000000000004E-7</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="I9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="11">
+        <v>1</v>
+      </c>
+      <c r="K9" s="11">
+        <v>0.35970000000000002</v>
+      </c>
+      <c r="L9" s="11">
+        <v>0.35970000000000002</v>
+      </c>
+      <c r="M9" s="11">
+        <v>18.739000000000001</v>
+      </c>
+      <c r="N9" s="15">
+        <v>2.7900000000000001E-5</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="14">
-        <v>1</v>
-      </c>
-      <c r="C10" s="14">
+      <c r="B10" s="11">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11">
         <v>0.91700000000000004</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="11">
         <v>0.91700000000000004</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="11">
         <v>5.9470000000000001</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="15">
         <v>1.5900000000000001E-2</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="I10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="11">
+        <v>1</v>
+      </c>
+      <c r="K10" s="11">
+        <v>8.48E-2</v>
+      </c>
+      <c r="L10" s="11">
+        <v>8.48E-2</v>
+      </c>
+      <c r="M10" s="11">
+        <v>4.4180000000000001</v>
+      </c>
+      <c r="N10" s="15">
+        <v>3.7310000000000003E-2</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="17">
         <v>145</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="17">
         <v>22.346</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="17">
         <v>0.154</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+      <c r="I11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="17">
+        <v>144</v>
+      </c>
+      <c r="K11" s="17">
+        <v>2.7641</v>
+      </c>
+      <c r="L11" s="17">
+        <v>1.9199999999999998E-2</v>
+      </c>
+      <c r="M11" s="17"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="18"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23" t="s">
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="53"/>
+      <c r="I12" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="53"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="19"/>
+      <c r="B13" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="21"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
+      <c r="G13" s="18"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="N13" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="O13" s="18"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="14">
+      <c r="B14" s="11">
+        <v>1</v>
+      </c>
+      <c r="C14" s="11">
         <v>0.86399999999999999</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="11">
         <v>0.86399999999999999</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="11">
         <v>4.1159999999999997</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="13">
         <v>4.4299999999999999E-2</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
+      <c r="I14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="11">
+        <v>1</v>
+      </c>
+      <c r="K14" s="11">
+        <v>3.39E-2</v>
+      </c>
+      <c r="L14" s="11">
+        <v>3.39E-2</v>
+      </c>
+      <c r="M14" s="11">
+        <v>1.9730000000000001</v>
+      </c>
+      <c r="N14" s="32">
+        <v>0.16225000000000001</v>
+      </c>
+      <c r="O14" s="7"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="14">
-        <v>1</v>
-      </c>
-      <c r="C15" s="14">
+      <c r="B15" s="11">
+        <v>1</v>
+      </c>
+      <c r="C15" s="11">
         <v>10.771000000000001</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="11">
         <v>10.771000000000001</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="11">
         <v>51.317999999999998</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="14">
         <v>3.6600000000000002E-11</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+      <c r="I15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="11">
+        <v>1</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0.1411</v>
+      </c>
+      <c r="L15" s="11">
+        <v>0.1411</v>
+      </c>
+      <c r="M15" s="11">
+        <v>8.2089999999999996</v>
+      </c>
+      <c r="N15" s="15">
+        <v>4.79E-3</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="14">
-        <v>1</v>
-      </c>
-      <c r="C16" s="31">
+      <c r="B16" s="11">
+        <v>1</v>
+      </c>
+      <c r="C16" s="25">
         <v>14.16</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="25">
         <v>14.16</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="11">
         <v>67.462000000000003</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="14">
         <v>1.0799999999999999E-13</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
+      <c r="I16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="11">
+        <v>1</v>
+      </c>
+      <c r="K16" s="24">
+        <v>0.1452</v>
+      </c>
+      <c r="L16" s="24">
+        <v>0.1452</v>
+      </c>
+      <c r="M16" s="11">
+        <v>8.4489999999999998</v>
+      </c>
+      <c r="N16" s="15">
+        <v>4.2300000000000003E-3</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="14">
-        <v>1</v>
-      </c>
-      <c r="C17" s="14">
+      <c r="B17" s="11">
+        <v>1</v>
+      </c>
+      <c r="C17" s="11">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="11">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="11">
         <v>1.6E-2</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="11">
         <v>0.90090000000000003</v>
       </c>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
+      <c r="I17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="11">
+        <v>1</v>
+      </c>
+      <c r="K17" s="11">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="L17" s="11">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="M17" s="11">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="N17" s="30">
+        <v>0.46461000000000002</v>
+      </c>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="14">
-        <v>1</v>
-      </c>
-      <c r="C18" s="14">
+      <c r="B18" s="11">
+        <v>1</v>
+      </c>
+      <c r="C18" s="11">
         <v>0.34499999999999997</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="11">
         <v>0.34499999999999997</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="11">
         <v>1.643</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="11">
         <v>0.2019</v>
       </c>
       <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
+      <c r="I18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="11">
+        <v>1</v>
+      </c>
+      <c r="K18" s="11">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="L18" s="11">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="M18" s="11">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="N18" s="30">
+        <v>0.70987999999999996</v>
+      </c>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="14">
-        <v>1</v>
-      </c>
-      <c r="C19" s="31">
+      <c r="B19" s="11">
+        <v>1</v>
+      </c>
+      <c r="C19" s="25">
         <v>5.68</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="25">
         <v>5.68</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="11">
         <v>27.062000000000001</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="14">
         <v>6.6000000000000003E-7</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+      <c r="I19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="11">
+        <v>1</v>
+      </c>
+      <c r="K19" s="24">
+        <v>0.33750000000000002</v>
+      </c>
+      <c r="L19" s="24">
+        <v>0.33750000000000002</v>
+      </c>
+      <c r="M19" s="11">
+        <v>19.634</v>
+      </c>
+      <c r="N19" s="14">
+        <v>1.8499999999999999E-5</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="14">
-        <v>1</v>
-      </c>
-      <c r="C20" s="14">
+      <c r="B20" s="11">
+        <v>1</v>
+      </c>
+      <c r="C20" s="11">
         <v>1.321</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="11">
         <v>1.321</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="11">
         <v>6.2949999999999999</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="15">
         <v>0.13200000000000001</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="I20" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="11">
+        <v>1</v>
+      </c>
+      <c r="K20" s="24">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="L20" s="24">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="M20" s="11">
+        <v>4.7709999999999999</v>
+      </c>
+      <c r="N20" s="15">
+        <v>3.0550000000000001E-2</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="17">
         <v>145</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="17">
         <v>30.434999999999999</v>
       </c>
-      <c r="D21" s="20">
-        <v>30.434999999999999</v>
-      </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="21"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
+      <c r="D21" s="36">
+        <v>0.21</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
+      <c r="I21" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="17">
+        <v>144</v>
+      </c>
+      <c r="K21" s="17">
+        <v>2.4750999999999999</v>
+      </c>
+      <c r="L21" s="17">
+        <v>1.72E-2</v>
+      </c>
+      <c r="M21" s="17"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="18"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23" t="s">
+      <c r="B22" s="52"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="53"/>
+      <c r="I22" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="53"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="19"/>
+      <c r="B23" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="23" t="s">
+      <c r="E23" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="21"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+      <c r="G23" s="18"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="M23" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="N23" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="O23" s="18"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="14">
-        <v>1</v>
-      </c>
-      <c r="C24" s="14">
+      <c r="B24" s="11">
+        <v>1</v>
+      </c>
+      <c r="C24" s="11">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="11">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="E24" s="31">
+      <c r="E24" s="25">
         <v>0.35</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="26">
         <v>0.55489599999999994</v>
       </c>
       <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
+      <c r="I24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="11">
+        <v>1</v>
+      </c>
+      <c r="K24" s="11">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L24" s="11">
+        <v>2.8E-3</v>
+      </c>
+      <c r="M24" s="25">
+        <v>0.109</v>
+      </c>
+      <c r="N24" s="32">
+        <v>0.74163000000000001</v>
+      </c>
+      <c r="O24" s="7"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="14">
-        <v>1</v>
-      </c>
-      <c r="C25" s="14">
+      <c r="B25" s="11">
+        <v>1</v>
+      </c>
+      <c r="C25" s="11">
         <v>0.1721</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="11">
         <v>0.1721</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="11">
         <v>18.870999999999999</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="14">
         <v>2.6100000000000001E-5</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
+      <c r="I25" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="11">
+        <v>1</v>
+      </c>
+      <c r="K25" s="25">
+        <v>0</v>
+      </c>
+      <c r="L25" s="24">
+        <v>0</v>
+      </c>
+      <c r="M25" s="25">
+        <v>0</v>
+      </c>
+      <c r="N25" s="32">
+        <v>0.99526999999999999</v>
+      </c>
+      <c r="O25" s="7"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="14">
-        <v>1</v>
-      </c>
-      <c r="C26" s="14">
+      <c r="B26" s="11">
+        <v>1</v>
+      </c>
+      <c r="C26" s="11">
         <v>0.65080000000000005</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="11">
         <v>0.65080000000000005</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="11">
         <v>71.337000000000003</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="14">
         <v>2.87E-14</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
+      <c r="I26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" s="11">
+        <v>1</v>
+      </c>
+      <c r="K26" s="11">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="L26" s="11">
+        <v>0.66439999999999999</v>
+      </c>
+      <c r="M26" s="25">
+        <v>26.14</v>
+      </c>
+      <c r="N26" s="14">
+        <v>9.95E-7</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="14">
-        <v>1</v>
-      </c>
-      <c r="C27" s="30">
+      <c r="B27" s="11">
+        <v>1</v>
+      </c>
+      <c r="C27" s="24">
         <v>0</v>
       </c>
-      <c r="D27" s="30">
+      <c r="D27" s="24">
         <v>0</v>
       </c>
-      <c r="E27" s="31">
+      <c r="E27" s="25">
         <v>0</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="11">
         <v>0.983707</v>
       </c>
       <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
+      <c r="I27" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="11">
+        <v>1</v>
+      </c>
+      <c r="K27" s="25">
+        <v>0</v>
+      </c>
+      <c r="L27" s="24">
+        <v>1E-4</v>
+      </c>
+      <c r="M27" s="25">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="N27" s="30">
+        <v>0.95967999999999998</v>
+      </c>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="14">
-        <v>1</v>
-      </c>
-      <c r="C28" s="14">
+      <c r="B28" s="11">
+        <v>1</v>
+      </c>
+      <c r="C28" s="11">
         <v>2.0799999999999999E-2</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="11">
         <v>2.0799999999999999E-2</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="11">
         <v>2.2810000000000001</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="11">
         <v>0.133106</v>
       </c>
       <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
+      <c r="I28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="11">
+        <v>1</v>
+      </c>
+      <c r="K28" s="11">
+        <v>1E-3</v>
+      </c>
+      <c r="L28" s="11">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="M28" s="11">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="N28" s="30">
+        <v>0.83845999999999998</v>
+      </c>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="14">
-        <v>1</v>
-      </c>
-      <c r="C29" s="14">
+      <c r="B29" s="11">
+        <v>1</v>
+      </c>
+      <c r="C29" s="11">
         <v>0.13619999999999999</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="11">
         <v>0.13619999999999999</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="11">
         <v>14.933999999999999</v>
       </c>
-      <c r="F29" s="17">
+      <c r="F29" s="14">
         <v>1.6699999999999999E-4</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
+      <c r="I29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" s="11">
+        <v>1</v>
+      </c>
+      <c r="K29" s="11">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="L29" s="24">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="M29" s="11">
+        <v>8.0649999999999995</v>
+      </c>
+      <c r="N29" s="15">
+        <v>5.1700000000000001E-3</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="14">
-        <v>1</v>
-      </c>
-      <c r="C30" s="14">
+      <c r="B30" s="11">
+        <v>1</v>
+      </c>
+      <c r="C30" s="11">
         <v>3.6900000000000002E-2</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="11">
         <v>3.6900000000000002E-2</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="11">
         <v>4.0439999999999996</v>
       </c>
-      <c r="F30" s="18">
+      <c r="F30" s="15">
         <v>4.6178999999999998E-2</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+      <c r="I30" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="11">
+        <v>1</v>
+      </c>
+      <c r="K30" s="25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L30" s="11">
+        <v>6.9699999999999998E-2</v>
+      </c>
+      <c r="M30" s="11">
+        <v>2.7429999999999999</v>
+      </c>
+      <c r="N30" s="32">
+        <v>9.9849999999999994E-2</v>
+      </c>
+      <c r="O30" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="12">
         <v>145</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="12">
         <v>1.3227</v>
       </c>
-      <c r="D31" s="15">
-        <v>1.3227</v>
-      </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
+      <c r="D31" s="12">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
       <c r="G31" s="3"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="I31" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31" s="17">
+        <v>144</v>
+      </c>
+      <c r="K31" s="38">
+        <v>3.66</v>
+      </c>
+      <c r="L31" s="12">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="M31" s="12"/>
+      <c r="N31" s="34"/>
+      <c r="O31" s="3"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
       <c r="B34">
         <v>20200903</v>
       </c>
+      <c r="I34" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="J34" s="28">
+        <v>20200904</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A12:G12"/>
     <mergeCell ref="A22:G22"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="I12:O12"/>
+    <mergeCell ref="I22:O22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C17842-2ED1-E849-B7EC-C33DC67EA4A3}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="39"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="56"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10">
+        <v>345.1</v>
+      </c>
+      <c r="D3" s="10">
+        <v>345.1</v>
+      </c>
+      <c r="E3" s="42">
+        <v>1014.47</v>
+      </c>
+      <c r="F3" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11">
+        <v>20.2</v>
+      </c>
+      <c r="D4" s="11">
+        <v>20.2</v>
+      </c>
+      <c r="E4" s="11">
+        <v>59.337000000000003</v>
+      </c>
+      <c r="F4" s="44">
+        <v>1.62E-14</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="11">
+        <v>15</v>
+      </c>
+      <c r="C5" s="11">
+        <v>431.4</v>
+      </c>
+      <c r="D5" s="11">
+        <v>28.8</v>
+      </c>
+      <c r="E5" s="11">
+        <v>84.536000000000001</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="11">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11">
+        <v>576.20000000000005</v>
+      </c>
+      <c r="D6" s="11">
+        <v>576.20000000000005</v>
+      </c>
+      <c r="E6" s="11">
+        <v>1693.5989999999999</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="11">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11">
+        <v>5.8</v>
+      </c>
+      <c r="D7" s="11">
+        <v>5.8</v>
+      </c>
+      <c r="E7" s="11">
+        <v>17.109000000000002</v>
+      </c>
+      <c r="F7" s="44">
+        <v>3.5899999999999998E-5</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="11">
+        <v>15</v>
+      </c>
+      <c r="C8" s="11">
+        <v>525.4</v>
+      </c>
+      <c r="D8" s="37">
+        <v>35</v>
+      </c>
+      <c r="E8" s="11">
+        <v>102.955</v>
+      </c>
+      <c r="F8" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="11">
+        <v>15</v>
+      </c>
+      <c r="C9" s="37">
+        <v>41</v>
+      </c>
+      <c r="D9" s="11">
+        <v>2.7</v>
+      </c>
+      <c r="E9" s="11">
+        <v>8.0380000000000003</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="11">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11">
+        <v>115.2</v>
+      </c>
+      <c r="D10" s="11">
+        <v>115.2</v>
+      </c>
+      <c r="E10" s="11">
+        <v>338.63499999999999</v>
+      </c>
+      <c r="F10" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="37">
+        <v>2</v>
+      </c>
+      <c r="D11" s="37">
+        <v>2</v>
+      </c>
+      <c r="E11" s="11">
+        <v>5.944</v>
+      </c>
+      <c r="F11" s="45">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="11">
+        <v>15</v>
+      </c>
+      <c r="C12" s="11">
+        <v>169.5</v>
+      </c>
+      <c r="D12" s="11">
+        <v>11.3</v>
+      </c>
+      <c r="E12" s="11">
+        <v>33.219000000000001</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="11">
+        <v>15</v>
+      </c>
+      <c r="C13" s="37">
+        <v>28.5</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1.9</v>
+      </c>
+      <c r="E13" s="11">
+        <v>5.593</v>
+      </c>
+      <c r="F13" s="44">
+        <v>1.7700000000000001E-11</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="11">
+        <v>1</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="11">
+        <v>1.579</v>
+      </c>
+      <c r="F14" s="46">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="11">
+        <v>15</v>
+      </c>
+      <c r="C15" s="37">
+        <v>170.2</v>
+      </c>
+      <c r="D15" s="11">
+        <v>11.3</v>
+      </c>
+      <c r="E15" s="11">
+        <v>33.347000000000001</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="11">
+        <v>15</v>
+      </c>
+      <c r="C16" s="11">
+        <v>26.7</v>
+      </c>
+      <c r="D16" s="11">
+        <v>1.8</v>
+      </c>
+      <c r="E16" s="11">
+        <v>5.242</v>
+      </c>
+      <c r="F16" s="44">
+        <v>1.57E-10</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="11">
+        <v>13</v>
+      </c>
+      <c r="C17" s="37">
+        <v>8.9</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="E17" s="11">
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="F17" s="45">
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="12">
+        <v>4554</v>
+      </c>
+      <c r="C18" s="12">
+        <v>1549.2</v>
+      </c>
+      <c r="D18" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B328694F-EA6E-604D-9A0B-A3FA03C0A0D4}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="56"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="10">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10">
+        <v>6.32</v>
+      </c>
+      <c r="D3" s="10">
+        <v>6.3220000000000001</v>
+      </c>
+      <c r="E3" s="42">
+        <v>43.956000000000003</v>
+      </c>
+      <c r="F3" s="58">
+        <v>5.6899999999999999E-11</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11">
+        <v>2.42</v>
+      </c>
+      <c r="D4" s="11">
+        <v>2.4169999999999998</v>
+      </c>
+      <c r="E4" s="11">
+        <v>16.803000000000001</v>
+      </c>
+      <c r="F4" s="44">
+        <v>4.5099999999999998E-5</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="11">
+        <v>8</v>
+      </c>
+      <c r="C5" s="11">
+        <v>16.02</v>
+      </c>
+      <c r="D5" s="11">
+        <v>2.0030000000000001</v>
+      </c>
+      <c r="E5" s="11">
+        <v>13.926</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="11">
+        <v>1</v>
+      </c>
+      <c r="C6" s="57">
+        <v>0.2</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="E6" s="11">
+        <v>1.3819999999999999</v>
+      </c>
+      <c r="F6" s="59">
+        <v>0.240069</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="11">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F7" s="60">
+        <v>0.71060100000000004</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="63" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="11">
+        <v>8</v>
+      </c>
+      <c r="C8" s="11">
+        <v>5.09</v>
+      </c>
+      <c r="D8" s="25">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="E8" s="11">
+        <v>4.4240000000000004</v>
+      </c>
+      <c r="F8" s="44">
+        <v>2.8500000000000002E-5</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="11">
+        <v>8</v>
+      </c>
+      <c r="C9" s="57">
+        <v>4.01</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0.502</v>
+      </c>
+      <c r="E9" s="11">
+        <v>3.488</v>
+      </c>
+      <c r="F9" s="45">
+        <v>5.6099999999999998E-4</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="11">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0.24</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="E10" s="11">
+        <v>1.6379999999999999</v>
+      </c>
+      <c r="F10" s="59">
+        <v>0.20089099999999999</v>
+      </c>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="57">
+        <v>0.17</v>
+      </c>
+      <c r="D11" s="25">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E11" s="11">
+        <v>1.216</v>
+      </c>
+      <c r="F11" s="59">
+        <v>0.27037099999999997</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="63" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="11">
+        <v>8</v>
+      </c>
+      <c r="C12" s="11">
+        <v>5.22</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="E12" s="11">
+        <v>4.5330000000000004</v>
+      </c>
+      <c r="F12" s="44">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="11">
+        <v>8</v>
+      </c>
+      <c r="C13" s="57">
+        <v>2.89</v>
+      </c>
+      <c r="D13" s="11">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="E13" s="11">
+        <v>2.5139999999999998</v>
+      </c>
+      <c r="F13" s="62">
+        <v>1.0481000000000001E-2</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="11">
+        <v>1</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0.46</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="E14" s="11">
+        <v>3.1829999999999998</v>
+      </c>
+      <c r="F14" s="46">
+        <v>7.4745000000000006E-2</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="11">
+        <v>6</v>
+      </c>
+      <c r="C15" s="57">
+        <v>0.75</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0.124</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="F15" s="59">
+        <v>0.52035699999999996</v>
+      </c>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="11">
+        <v>8</v>
+      </c>
+      <c r="C16" s="11">
+        <v>1.84</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="E16" s="11">
+        <v>1.595</v>
+      </c>
+      <c r="F16" s="61">
+        <v>0.12207999999999999</v>
+      </c>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="11">
+        <v>4</v>
+      </c>
+      <c r="C17" s="57">
+        <v>0.26</v>
+      </c>
+      <c r="D17" s="11">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="F17" s="59">
+        <v>0.76642500000000002</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="12">
+        <v>929</v>
+      </c>
+      <c r="C18" s="12">
+        <v>133.62</v>
+      </c>
+      <c r="D18" s="12">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54CD5EF-8E5E-5545-8C70-9F4575832390}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD30523-03A2-2C4D-896D-A99246512D08}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{868754AE-9F6B-044A-B870-E062F6FE947C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB99170-34EF-B643-AA40-08FFACE5F84C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A9BAF9-FBD3-4846-B869-92903463ECCA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>